<commit_message>
[Update] Changed Expense and Income download to allow for periods and start/end dates
</commit_message>
<xml_diff>
--- a/backend/income_details.xlsx
+++ b/backend/income_details.xlsx
@@ -421,21 +421,21 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Salary</v>
+        <v>subway</v>
       </c>
       <c r="B2">
-        <v>600</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1">
-        <v>45799.45483353009</v>
+        <v>45799.333333333336</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>subway</v>
+        <v>Salary</v>
       </c>
       <c r="B3">
-        <v>12</v>
+        <v>600</v>
       </c>
       <c r="C3" s="1">
         <v>45799.333333333336</v>

</xml_diff>